<commit_message>
Atualização excel backlog - requisito desejavel
</commit_message>
<xml_diff>
--- a/private/Backlog/backologDisney.xlsx
+++ b/private/Backlog/backologDisney.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natta\OneDrive\Área de Trabalho\CCOK\PROJETO INDIVIDUAL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natta\OneDrive\Área de Trabalho\CCOK\PROJETO INDIVIDUAL\ProjetoIndividual-DisneyPrincess\private\Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A332321F-B6EC-4393-A80E-8A0620E24ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD16873E-A190-497B-A0A1-02208D00B4AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6ECB3DF9-783C-432F-AE05-9A2DE3096434}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="backlog" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$B$1:$AE$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">backlog!$B$1:$AE$15</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="49">
   <si>
     <t>Requisito</t>
   </si>
@@ -159,6 +159,33 @@
   </si>
   <si>
     <t>SP3B</t>
+  </si>
+  <si>
+    <t>Playlist Princesas no site</t>
+  </si>
+  <si>
+    <t>Adcionar Playlists das princesas no site</t>
+  </si>
+  <si>
+    <t>Desejavel</t>
+  </si>
+  <si>
+    <t>Adcionar calculos aprendidos em Arq Comp</t>
+  </si>
+  <si>
+    <t>Inserir o BD dentro da VM</t>
+  </si>
+  <si>
+    <t>Escolher as ODS pertecentes ao projeto</t>
+  </si>
+  <si>
+    <t>Aplicar conceitos aprendidos em aula no projeto</t>
+  </si>
+  <si>
+    <t>Utilizar a API no cadastro do site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Realizar um diagrama de solução tecnica </t>
   </si>
 </sst>
 </file>
@@ -261,7 +288,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -391,19 +418,6 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -519,21 +533,65 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -543,6 +601,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -552,112 +616,49 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -737,7 +738,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Planilha1!$AG$2</c:f>
+              <c:f>backlog!$AG$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -772,7 +773,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$AJ$2:$AM$2</c:f>
+              <c:f>backlog!$AJ$2:$AM$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -797,7 +798,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Planilha1!$AG$3</c:f>
+              <c:f>backlog!$AG$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -832,7 +833,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$AJ$3:$AM$3</c:f>
+              <c:f>backlog!$AJ$3:$AM$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1957,79 +1958,79 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{884691E7-DAB8-4DFD-826C-65D96ECBE77D}">
   <dimension ref="A1:AM37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="43" workbookViewId="0">
-      <selection activeCell="AI26" sqref="AI26"/>
+    <sheetView tabSelected="1" zoomScale="68" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18" style="5" customWidth="1"/>
-    <col min="2" max="2" width="13.21875" style="5" customWidth="1"/>
-    <col min="3" max="6" width="8.88671875" style="5"/>
+    <col min="1" max="1" width="18" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.77734375" style="1" customWidth="1"/>
+    <col min="3" max="6" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:39" ht="21" x14ac:dyDescent="0.4">
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34" t="s">
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="34"/>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="34"/>
-      <c r="X1" s="34" t="s">
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44"/>
+      <c r="R1" s="44"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="44"/>
+      <c r="U1" s="44"/>
+      <c r="V1" s="44"/>
+      <c r="W1" s="44"/>
+      <c r="X1" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="Y1" s="34"/>
-      <c r="Z1" s="34"/>
-      <c r="AA1" s="34" t="s">
+      <c r="Y1" s="44"/>
+      <c r="Z1" s="44"/>
+      <c r="AA1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="AB1" s="34"/>
-      <c r="AC1" s="34" t="s">
+      <c r="AB1" s="44"/>
+      <c r="AC1" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="AD1" s="34"/>
-      <c r="AE1" s="31" t="s">
+      <c r="AD1" s="44"/>
+      <c r="AE1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="AF1" s="29"/>
-      <c r="AG1" s="22" t="s">
+      <c r="AF1" s="4"/>
+      <c r="AG1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AH1" s="21" t="s">
+      <c r="AH1" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="AI1" s="21"/>
-      <c r="AJ1" s="17" t="s">
+      <c r="AI1" s="10"/>
+      <c r="AJ1" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="AK1" s="17"/>
-      <c r="AL1" s="18" t="s">
+      <c r="AK1" s="43"/>
+      <c r="AL1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="AM1" s="18"/>
+      <c r="AM1" s="9"/>
     </row>
     <row r="2" spans="2:39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="34" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="35"/>
@@ -2064,890 +2065,878 @@
         <v>10</v>
       </c>
       <c r="AB2" s="41"/>
-      <c r="AC2" s="32">
+      <c r="AC2" s="42">
         <v>13</v>
       </c>
-      <c r="AD2" s="33"/>
-      <c r="AE2" s="42" t="s">
+      <c r="AD2" s="34"/>
+      <c r="AE2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="AG2" s="23" t="s">
+      <c r="AG2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AH2" s="19">
+      <c r="AH2" s="7">
         <f>SUM(AC2:AD15)</f>
         <v>154</v>
       </c>
-      <c r="AI2" s="20"/>
-      <c r="AJ2" s="19">
+      <c r="AI2" s="8"/>
+      <c r="AJ2" s="7">
         <v>100</v>
       </c>
-      <c r="AK2" s="20"/>
-      <c r="AL2" s="19">
+      <c r="AK2" s="8"/>
+      <c r="AL2" s="7">
         <v>54</v>
       </c>
-      <c r="AM2" s="20"/>
+      <c r="AM2" s="8"/>
     </row>
     <row r="3" spans="2:39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="6" t="s">
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="13" t="s">
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="23"/>
+      <c r="U3" s="23"/>
+      <c r="V3" s="23"/>
+      <c r="W3" s="24"/>
+      <c r="X3" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="Y3" s="13"/>
-      <c r="Z3" s="13"/>
-      <c r="AA3" s="24" t="s">
+      <c r="Y3" s="30"/>
+      <c r="Z3" s="30"/>
+      <c r="AA3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="AB3" s="24"/>
-      <c r="AC3" s="27">
+      <c r="AB3" s="25"/>
+      <c r="AC3" s="26">
         <v>5</v>
       </c>
-      <c r="AD3" s="9"/>
-      <c r="AE3" s="42" t="s">
+      <c r="AD3" s="27"/>
+      <c r="AE3" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="AG3" s="23" t="s">
+      <c r="AG3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AH3" s="19">
+      <c r="AH3" s="7">
         <f>SUM(AC8,AC9,AC11,AC13)</f>
         <v>47</v>
       </c>
-      <c r="AI3" s="20"/>
-      <c r="AJ3" s="19">
+      <c r="AI3" s="8"/>
+      <c r="AJ3" s="7">
         <v>40</v>
       </c>
-      <c r="AK3" s="20"/>
-      <c r="AL3" s="19">
+      <c r="AK3" s="8"/>
+      <c r="AL3" s="7">
         <v>7</v>
       </c>
-      <c r="AM3" s="20"/>
+      <c r="AM3" s="8"/>
     </row>
     <row r="4" spans="2:39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="6" t="s">
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7"/>
-      <c r="U4" s="7"/>
-      <c r="V4" s="7"/>
-      <c r="W4" s="8"/>
-      <c r="X4" s="13" t="s">
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="23"/>
+      <c r="U4" s="23"/>
+      <c r="V4" s="23"/>
+      <c r="W4" s="24"/>
+      <c r="X4" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="Y4" s="13"/>
-      <c r="Z4" s="13"/>
-      <c r="AA4" s="24" t="s">
+      <c r="Y4" s="30"/>
+      <c r="Z4" s="30"/>
+      <c r="AA4" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="AB4" s="24"/>
-      <c r="AC4" s="27">
+      <c r="AB4" s="25"/>
+      <c r="AC4" s="26">
         <v>13</v>
       </c>
-      <c r="AD4" s="9"/>
-      <c r="AE4" s="42" t="s">
+      <c r="AD4" s="27"/>
+      <c r="AE4" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="AG4" s="23" t="s">
+      <c r="AG4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AH4" s="47">
+      <c r="AH4" s="31">
         <f>SUM(AH2:AI3)</f>
         <v>201</v>
       </c>
-      <c r="AI4" s="48"/>
-      <c r="AJ4" s="48"/>
-      <c r="AK4" s="48"/>
-      <c r="AL4" s="48"/>
-      <c r="AM4" s="49"/>
+      <c r="AI4" s="32"/>
+      <c r="AJ4" s="32"/>
+      <c r="AK4" s="32"/>
+      <c r="AL4" s="32"/>
+      <c r="AM4" s="33"/>
     </row>
     <row r="5" spans="2:39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="6" t="s">
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
-      <c r="W5" s="8"/>
-      <c r="X5" s="13" t="s">
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
+      <c r="U5" s="23"/>
+      <c r="V5" s="23"/>
+      <c r="W5" s="24"/>
+      <c r="X5" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="Y5" s="13"/>
-      <c r="Z5" s="13"/>
-      <c r="AA5" s="24" t="s">
+      <c r="Y5" s="30"/>
+      <c r="Z5" s="30"/>
+      <c r="AA5" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="AB5" s="24"/>
-      <c r="AC5" s="27">
+      <c r="AB5" s="25"/>
+      <c r="AC5" s="26">
         <v>13</v>
       </c>
-      <c r="AD5" s="9"/>
-      <c r="AE5" s="42" t="s">
+      <c r="AD5" s="27"/>
+      <c r="AE5" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="6" spans="2:39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="6" t="s">
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7"/>
-      <c r="U6" s="7"/>
-      <c r="V6" s="7"/>
-      <c r="W6" s="8"/>
-      <c r="X6" s="13" t="s">
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="23"/>
+      <c r="T6" s="23"/>
+      <c r="U6" s="23"/>
+      <c r="V6" s="23"/>
+      <c r="W6" s="24"/>
+      <c r="X6" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="Y6" s="13"/>
-      <c r="Z6" s="13"/>
-      <c r="AA6" s="24" t="s">
+      <c r="Y6" s="30"/>
+      <c r="Z6" s="30"/>
+      <c r="AA6" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="AB6" s="24"/>
-      <c r="AC6" s="27">
+      <c r="AB6" s="25"/>
+      <c r="AC6" s="26">
         <v>13</v>
       </c>
-      <c r="AD6" s="9"/>
-      <c r="AE6" s="42" t="s">
+      <c r="AD6" s="27"/>
+      <c r="AE6" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="7" spans="2:39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="6" t="s">
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7"/>
-      <c r="U7" s="7"/>
-      <c r="V7" s="7"/>
-      <c r="W7" s="8"/>
-      <c r="X7" s="13" t="s">
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="23"/>
+      <c r="U7" s="23"/>
+      <c r="V7" s="23"/>
+      <c r="W7" s="24"/>
+      <c r="X7" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="Y7" s="13"/>
-      <c r="Z7" s="13"/>
-      <c r="AA7" s="24" t="s">
+      <c r="Y7" s="30"/>
+      <c r="Z7" s="30"/>
+      <c r="AA7" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="AB7" s="24"/>
-      <c r="AC7" s="27">
+      <c r="AB7" s="25"/>
+      <c r="AC7" s="26">
         <v>21</v>
       </c>
-      <c r="AD7" s="9"/>
-      <c r="AE7" s="42" t="s">
+      <c r="AD7" s="27"/>
+      <c r="AE7" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="8" spans="2:39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
-      <c r="U8" s="7"/>
-      <c r="V8" s="7"/>
-      <c r="W8" s="8"/>
-      <c r="X8" s="13" t="s">
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="23"/>
+      <c r="S8" s="23"/>
+      <c r="T8" s="23"/>
+      <c r="U8" s="23"/>
+      <c r="V8" s="23"/>
+      <c r="W8" s="24"/>
+      <c r="X8" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="Y8" s="13"/>
-      <c r="Z8" s="13"/>
-      <c r="AA8" s="24" t="s">
+      <c r="Y8" s="30"/>
+      <c r="Z8" s="30"/>
+      <c r="AA8" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AB8" s="24"/>
-      <c r="AC8" s="27">
+      <c r="AB8" s="25"/>
+      <c r="AC8" s="26">
         <v>8</v>
       </c>
-      <c r="AD8" s="9"/>
-      <c r="AE8" s="42" t="s">
+      <c r="AD8" s="27"/>
+      <c r="AE8" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="9" spans="2:39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="7"/>
-      <c r="U9" s="7"/>
-      <c r="V9" s="7"/>
-      <c r="W9" s="8"/>
-      <c r="X9" s="13" t="s">
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="23"/>
+      <c r="R9" s="23"/>
+      <c r="S9" s="23"/>
+      <c r="T9" s="23"/>
+      <c r="U9" s="23"/>
+      <c r="V9" s="23"/>
+      <c r="W9" s="24"/>
+      <c r="X9" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="Y9" s="13"/>
-      <c r="Z9" s="13"/>
-      <c r="AA9" s="24" t="s">
+      <c r="Y9" s="30"/>
+      <c r="Z9" s="30"/>
+      <c r="AA9" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="AB9" s="24"/>
-      <c r="AC9" s="27">
+      <c r="AB9" s="25"/>
+      <c r="AC9" s="26">
         <v>13</v>
       </c>
-      <c r="AD9" s="9"/>
-      <c r="AE9" s="42" t="s">
+      <c r="AD9" s="27"/>
+      <c r="AE9" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="10" spans="2:39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
-      <c r="T10" s="7"/>
-      <c r="U10" s="7"/>
-      <c r="V10" s="7"/>
-      <c r="W10" s="8"/>
-      <c r="X10" s="13" t="s">
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="23"/>
+      <c r="Q10" s="23"/>
+      <c r="R10" s="23"/>
+      <c r="S10" s="23"/>
+      <c r="T10" s="23"/>
+      <c r="U10" s="23"/>
+      <c r="V10" s="23"/>
+      <c r="W10" s="24"/>
+      <c r="X10" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="Y10" s="13"/>
-      <c r="Z10" s="13"/>
-      <c r="AA10" s="24" t="s">
+      <c r="Y10" s="30"/>
+      <c r="Z10" s="30"/>
+      <c r="AA10" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="AB10" s="24"/>
-      <c r="AC10" s="27">
+      <c r="AB10" s="25"/>
+      <c r="AC10" s="26">
         <v>5</v>
       </c>
-      <c r="AD10" s="9"/>
-      <c r="AE10" s="42" t="s">
+      <c r="AD10" s="27"/>
+      <c r="AE10" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="11" spans="2:39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
-      <c r="S11" s="7"/>
-      <c r="T11" s="7"/>
-      <c r="U11" s="7"/>
-      <c r="V11" s="7"/>
-      <c r="W11" s="8"/>
-      <c r="X11" s="13" t="s">
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
+      <c r="Q11" s="23"/>
+      <c r="R11" s="23"/>
+      <c r="S11" s="23"/>
+      <c r="T11" s="23"/>
+      <c r="U11" s="23"/>
+      <c r="V11" s="23"/>
+      <c r="W11" s="24"/>
+      <c r="X11" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="Y11" s="13"/>
-      <c r="Z11" s="13"/>
-      <c r="AA11" s="24" t="s">
+      <c r="Y11" s="30"/>
+      <c r="Z11" s="30"/>
+      <c r="AA11" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="AB11" s="24"/>
-      <c r="AC11" s="27">
+      <c r="AB11" s="25"/>
+      <c r="AC11" s="26">
         <v>13</v>
       </c>
-      <c r="AD11" s="9"/>
-      <c r="AE11" s="42" t="s">
+      <c r="AD11" s="27"/>
+      <c r="AE11" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" spans="2:39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="6" t="s">
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
-      <c r="S12" s="7"/>
-      <c r="T12" s="7"/>
-      <c r="U12" s="7"/>
-      <c r="V12" s="7"/>
-      <c r="W12" s="8"/>
-      <c r="X12" s="13" t="s">
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23"/>
+      <c r="Q12" s="23"/>
+      <c r="R12" s="23"/>
+      <c r="S12" s="23"/>
+      <c r="T12" s="23"/>
+      <c r="U12" s="23"/>
+      <c r="V12" s="23"/>
+      <c r="W12" s="24"/>
+      <c r="X12" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="Y12" s="13"/>
-      <c r="Z12" s="13"/>
-      <c r="AA12" s="24" t="s">
+      <c r="Y12" s="30"/>
+      <c r="Z12" s="30"/>
+      <c r="AA12" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AB12" s="24"/>
-      <c r="AC12" s="27">
+      <c r="AB12" s="25"/>
+      <c r="AC12" s="26">
         <v>8</v>
       </c>
-      <c r="AD12" s="9"/>
-      <c r="AE12" s="42" t="s">
+      <c r="AD12" s="27"/>
+      <c r="AE12" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="13" spans="2:39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="7"/>
-      <c r="S13" s="7"/>
-      <c r="T13" s="7"/>
-      <c r="U13" s="7"/>
-      <c r="V13" s="7"/>
-      <c r="W13" s="8"/>
-      <c r="X13" s="13" t="s">
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="23"/>
+      <c r="Q13" s="23"/>
+      <c r="R13" s="23"/>
+      <c r="S13" s="23"/>
+      <c r="T13" s="23"/>
+      <c r="U13" s="23"/>
+      <c r="V13" s="23"/>
+      <c r="W13" s="24"/>
+      <c r="X13" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="Y13" s="13"/>
-      <c r="Z13" s="13"/>
-      <c r="AA13" s="24" t="s">
+      <c r="Y13" s="30"/>
+      <c r="Z13" s="30"/>
+      <c r="AA13" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="AB13" s="24"/>
-      <c r="AC13" s="27">
+      <c r="AB13" s="25"/>
+      <c r="AC13" s="26">
         <v>13</v>
       </c>
-      <c r="AD13" s="9"/>
-      <c r="AE13" s="42" t="s">
+      <c r="AD13" s="27"/>
+      <c r="AE13" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="14" spans="2:39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="6" t="s">
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="7"/>
-      <c r="R14" s="7"/>
-      <c r="S14" s="7"/>
-      <c r="T14" s="7"/>
-      <c r="U14" s="7"/>
-      <c r="V14" s="7"/>
-      <c r="W14" s="8"/>
-      <c r="X14" s="13" t="s">
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="23"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="23"/>
+      <c r="Q14" s="23"/>
+      <c r="R14" s="23"/>
+      <c r="S14" s="23"/>
+      <c r="T14" s="23"/>
+      <c r="U14" s="23"/>
+      <c r="V14" s="23"/>
+      <c r="W14" s="24"/>
+      <c r="X14" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="Y14" s="13"/>
-      <c r="Z14" s="13"/>
-      <c r="AA14" s="24" t="s">
+      <c r="Y14" s="30"/>
+      <c r="Z14" s="30"/>
+      <c r="AA14" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AB14" s="24"/>
-      <c r="AC14" s="27">
+      <c r="AB14" s="25"/>
+      <c r="AC14" s="26">
         <v>8</v>
       </c>
-      <c r="AD14" s="9"/>
-      <c r="AE14" s="42" t="s">
+      <c r="AD14" s="27"/>
+      <c r="AE14" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="15" spans="2:39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
-      <c r="T15" s="7"/>
-      <c r="U15" s="7"/>
-      <c r="V15" s="7"/>
-      <c r="W15" s="8"/>
-      <c r="X15" s="13" t="s">
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="23"/>
+      <c r="Q15" s="23"/>
+      <c r="R15" s="23"/>
+      <c r="S15" s="23"/>
+      <c r="T15" s="23"/>
+      <c r="U15" s="23"/>
+      <c r="V15" s="23"/>
+      <c r="W15" s="24"/>
+      <c r="X15" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="Y15" s="13"/>
-      <c r="Z15" s="13"/>
-      <c r="AA15" s="24" t="s">
+      <c r="Y15" s="30"/>
+      <c r="Z15" s="30"/>
+      <c r="AA15" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AB15" s="24"/>
-      <c r="AC15" s="27">
+      <c r="AB15" s="25"/>
+      <c r="AC15" s="26">
         <v>8</v>
       </c>
-      <c r="AD15" s="9"/>
-      <c r="AE15" s="42" t="s">
+      <c r="AD15" s="27"/>
+      <c r="AE15" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="16" spans="2:39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="9"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="7"/>
-      <c r="S16" s="7"/>
-      <c r="T16" s="7"/>
-      <c r="U16" s="7"/>
-      <c r="V16" s="7"/>
-      <c r="W16" s="8"/>
-      <c r="X16" s="14"/>
-      <c r="Y16" s="14"/>
-      <c r="Z16" s="14"/>
-      <c r="AA16" s="24"/>
-      <c r="AB16" s="24"/>
-      <c r="AC16" s="27"/>
-      <c r="AD16" s="9"/>
-      <c r="AE16" s="42"/>
+      <c r="B16" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="23"/>
+      <c r="Q16" s="23"/>
+      <c r="R16" s="23"/>
+      <c r="S16" s="23"/>
+      <c r="T16" s="23"/>
+      <c r="U16" s="23"/>
+      <c r="V16" s="23"/>
+      <c r="W16" s="24"/>
+      <c r="X16" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y16" s="30"/>
+      <c r="Z16" s="30"/>
+      <c r="AA16" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB16" s="25"/>
+      <c r="AC16" s="26">
+        <v>8</v>
+      </c>
+      <c r="AD16" s="27"/>
+      <c r="AE16" s="6" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="17" spans="1:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="43"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="7"/>
-      <c r="S17" s="7"/>
-      <c r="T17" s="7"/>
-      <c r="U17" s="7"/>
-      <c r="V17" s="7"/>
-      <c r="W17" s="8"/>
-      <c r="X17" s="15"/>
-      <c r="Y17" s="15"/>
-      <c r="Z17" s="15"/>
-      <c r="AA17" s="24"/>
-      <c r="AB17" s="24"/>
-      <c r="AC17" s="27"/>
-      <c r="AD17" s="9"/>
-      <c r="AE17" s="42"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="23"/>
+      <c r="P17" s="23"/>
+      <c r="Q17" s="23"/>
+      <c r="R17" s="23"/>
+      <c r="S17" s="23"/>
+      <c r="T17" s="23"/>
+      <c r="U17" s="23"/>
+      <c r="V17" s="23"/>
+      <c r="W17" s="24"/>
+      <c r="X17" s="30"/>
+      <c r="Y17" s="30"/>
+      <c r="Z17" s="30"/>
+      <c r="AA17" s="25"/>
+      <c r="AB17" s="25"/>
+      <c r="AC17" s="26"/>
+      <c r="AD17" s="27"/>
+      <c r="AE17" s="6"/>
     </row>
     <row r="18" spans="1:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
-      <c r="B18" s="46"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
-      <c r="O18" s="12"/>
-      <c r="P18" s="12"/>
-      <c r="Q18" s="12"/>
-      <c r="R18" s="12"/>
-      <c r="S18" s="12"/>
-      <c r="T18" s="12"/>
-      <c r="U18" s="12"/>
-      <c r="V18" s="12"/>
-      <c r="W18" s="12"/>
-      <c r="X18" s="16"/>
-      <c r="Y18" s="16"/>
-      <c r="Z18" s="16"/>
-      <c r="AA18" s="25"/>
-      <c r="AB18" s="26"/>
-      <c r="AC18" s="28"/>
-      <c r="AD18" s="30"/>
-      <c r="AE18" s="42"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="14"/>
+      <c r="U18" s="14"/>
+      <c r="V18" s="14"/>
+      <c r="W18" s="14"/>
+      <c r="X18" s="30"/>
+      <c r="Y18" s="30"/>
+      <c r="Z18" s="30"/>
+      <c r="AA18" s="15"/>
+      <c r="AB18" s="16"/>
+      <c r="AC18" s="17"/>
+      <c r="AD18" s="18"/>
+      <c r="AE18" s="6"/>
     </row>
     <row r="19" spans="1:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
-      <c r="T19" s="1"/>
-      <c r="U19" s="1"/>
-      <c r="V19" s="1"/>
-      <c r="W19" s="2"/>
-      <c r="X19" s="2"/>
-      <c r="Y19" s="2"/>
-      <c r="Z19" s="1"/>
-      <c r="AA19" s="1"/>
-      <c r="AB19" s="1"/>
-      <c r="AC19" s="1"/>
+      <c r="A19"/>
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="11"/>
+      <c r="T19" s="11"/>
+      <c r="U19" s="11"/>
+      <c r="V19" s="11"/>
+      <c r="W19" s="12"/>
+      <c r="X19" s="12"/>
+      <c r="Y19" s="12"/>
+      <c r="Z19" s="11"/>
+      <c r="AA19" s="11"/>
+      <c r="AB19" s="11"/>
+      <c r="AC19" s="11"/>
     </row>
     <row r="20" spans="1:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
+      <c r="A20"/>
+      <c r="B20"/>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="F20"/>
     </row>
     <row r="21" spans="1:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
+      <c r="A21"/>
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21"/>
     </row>
     <row r="22" spans="1:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
+      <c r="A22"/>
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
     </row>
     <row r="23" spans="1:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
+      <c r="A23"/>
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
     </row>
     <row r="24" spans="1:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
+      <c r="A24"/>
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
     </row>
     <row r="25" spans="1:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
+      <c r="A25"/>
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
     </row>
     <row r="26" spans="1:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
+      <c r="A26"/>
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26"/>
+      <c r="F26"/>
     </row>
     <row r="27" spans="1:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
+      <c r="A27"/>
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="F27"/>
     </row>
     <row r="28" spans="1:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
+      <c r="A28"/>
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="F28"/>
     </row>
     <row r="29" spans="1:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
+      <c r="A29"/>
+      <c r="B29"/>
+      <c r="C29"/>
+      <c r="D29"/>
+      <c r="E29"/>
+      <c r="F29"/>
     </row>
     <row r="30" spans="1:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
+      <c r="A30"/>
+      <c r="B30"/>
+      <c r="C30"/>
+      <c r="D30"/>
+      <c r="E30"/>
+      <c r="F30"/>
     </row>
     <row r="31" spans="1:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
+      <c r="A31"/>
+      <c r="B31"/>
+      <c r="C31"/>
+      <c r="D31"/>
+      <c r="E31"/>
+      <c r="F31"/>
     </row>
     <row r="32" spans="1:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-    </row>
-    <row r="33" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-    </row>
-    <row r="34" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-    </row>
+      <c r="A32"/>
+      <c r="B32"/>
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="E32"/>
+      <c r="F32"/>
+    </row>
+    <row r="33" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="37" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <autoFilter ref="B1:AE15" xr:uid="{884691E7-DAB8-4DFD-826C-65D96ECBE77D}">
     <filterColumn colId="0" showButton="0"/>
@@ -2976,6 +2965,86 @@
     <filterColumn colId="27" showButton="0"/>
   </autoFilter>
   <mergeCells count="104">
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:W2"/>
+    <mergeCell ref="X2:Z2"/>
+    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="AC2:AD2"/>
+    <mergeCell ref="AJ1:AK1"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="H1:W1"/>
+    <mergeCell ref="X1:Z1"/>
+    <mergeCell ref="AA1:AB1"/>
+    <mergeCell ref="AC1:AD1"/>
+    <mergeCell ref="AH4:AM4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="H5:W5"/>
+    <mergeCell ref="X5:Z5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AH3:AI3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="H4:W4"/>
+    <mergeCell ref="X4:Z4"/>
+    <mergeCell ref="AA4:AB4"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="AJ3:AK3"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="H3:W3"/>
+    <mergeCell ref="X3:Z3"/>
+    <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="AC3:AD3"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="H7:W7"/>
+    <mergeCell ref="X7:Z7"/>
+    <mergeCell ref="AA7:AB7"/>
+    <mergeCell ref="AC7:AD7"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="H6:W6"/>
+    <mergeCell ref="X6:Z6"/>
+    <mergeCell ref="AA6:AB6"/>
+    <mergeCell ref="AC6:AD6"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="H9:W9"/>
+    <mergeCell ref="X9:Z9"/>
+    <mergeCell ref="AA9:AB9"/>
+    <mergeCell ref="AC9:AD9"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="H8:W8"/>
+    <mergeCell ref="X8:Z8"/>
+    <mergeCell ref="AA8:AB8"/>
+    <mergeCell ref="AC8:AD8"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="H11:W11"/>
+    <mergeCell ref="X11:Z11"/>
+    <mergeCell ref="AA11:AB11"/>
+    <mergeCell ref="AC11:AD11"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="H10:W10"/>
+    <mergeCell ref="X10:Z10"/>
+    <mergeCell ref="AA10:AB10"/>
+    <mergeCell ref="AC10:AD10"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="H13:W13"/>
+    <mergeCell ref="X13:Z13"/>
+    <mergeCell ref="AA13:AB13"/>
+    <mergeCell ref="AC13:AD13"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="H12:W12"/>
+    <mergeCell ref="X12:Z12"/>
+    <mergeCell ref="AA12:AB12"/>
+    <mergeCell ref="AC12:AD12"/>
+    <mergeCell ref="AC16:AD16"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="H15:W15"/>
+    <mergeCell ref="X15:Z15"/>
+    <mergeCell ref="AA15:AB15"/>
+    <mergeCell ref="AC15:AD15"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="H14:W14"/>
+    <mergeCell ref="X14:Z14"/>
+    <mergeCell ref="AA14:AB14"/>
+    <mergeCell ref="AC14:AD14"/>
     <mergeCell ref="AL3:AM3"/>
     <mergeCell ref="AL1:AM1"/>
     <mergeCell ref="AH2:AI2"/>
@@ -3000,86 +3069,6 @@
     <mergeCell ref="H16:W16"/>
     <mergeCell ref="X16:Z16"/>
     <mergeCell ref="AA16:AB16"/>
-    <mergeCell ref="AC16:AD16"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="H15:W15"/>
-    <mergeCell ref="X15:Z15"/>
-    <mergeCell ref="AA15:AB15"/>
-    <mergeCell ref="AC15:AD15"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="H14:W14"/>
-    <mergeCell ref="X14:Z14"/>
-    <mergeCell ref="AA14:AB14"/>
-    <mergeCell ref="AC14:AD14"/>
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="H13:W13"/>
-    <mergeCell ref="X13:Z13"/>
-    <mergeCell ref="AA13:AB13"/>
-    <mergeCell ref="AC13:AD13"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="H12:W12"/>
-    <mergeCell ref="X12:Z12"/>
-    <mergeCell ref="AA12:AB12"/>
-    <mergeCell ref="AC12:AD12"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="H11:W11"/>
-    <mergeCell ref="X11:Z11"/>
-    <mergeCell ref="AA11:AB11"/>
-    <mergeCell ref="AC11:AD11"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="H10:W10"/>
-    <mergeCell ref="X10:Z10"/>
-    <mergeCell ref="AA10:AB10"/>
-    <mergeCell ref="AC10:AD10"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="H9:W9"/>
-    <mergeCell ref="X9:Z9"/>
-    <mergeCell ref="AA9:AB9"/>
-    <mergeCell ref="AC9:AD9"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="H8:W8"/>
-    <mergeCell ref="X8:Z8"/>
-    <mergeCell ref="AA8:AB8"/>
-    <mergeCell ref="AC8:AD8"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="H7:W7"/>
-    <mergeCell ref="X7:Z7"/>
-    <mergeCell ref="AA7:AB7"/>
-    <mergeCell ref="AC7:AD7"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="H6:W6"/>
-    <mergeCell ref="X6:Z6"/>
-    <mergeCell ref="AA6:AB6"/>
-    <mergeCell ref="AC6:AD6"/>
-    <mergeCell ref="AH4:AM4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="H5:W5"/>
-    <mergeCell ref="X5:Z5"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="AH3:AI3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="H4:W4"/>
-    <mergeCell ref="X4:Z4"/>
-    <mergeCell ref="AA4:AB4"/>
-    <mergeCell ref="AC4:AD4"/>
-    <mergeCell ref="AJ3:AK3"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="H3:W3"/>
-    <mergeCell ref="X3:Z3"/>
-    <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="AC3:AD3"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:W2"/>
-    <mergeCell ref="X2:Z2"/>
-    <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="AJ1:AK1"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="H1:W1"/>
-    <mergeCell ref="X1:Z1"/>
-    <mergeCell ref="AA1:AB1"/>
-    <mergeCell ref="AC1:AD1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>